<commit_message>
update - extra data
</commit_message>
<xml_diff>
--- a/DSLSpeedTestData.xlsx
+++ b/DSLSpeedTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="35">
   <si>
     <t>LAN</t>
   </si>
@@ -119,6 +119,12 @@
   <si>
     <t>24.01.2016</t>
   </si>
+  <si>
+    <t>27.01.2016</t>
+  </si>
+  <si>
+    <t>28.01.2016</t>
+  </si>
 </sst>
 </file>
 
@@ -173,7 +179,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="339">
+  <cellStyleXfs count="367">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -513,8 +519,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -535,8 +569,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="339">
+  <cellStyles count="367">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -706,6 +741,20 @@
     <cellStyle name="Besuchter Link" xfId="334" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="336" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="364" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="366" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -875,6 +924,20 @@
     <cellStyle name="Link" xfId="333" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="335" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="363" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="365" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1204,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I255"/>
+  <dimension ref="A1:I275"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A230" workbookViewId="0">
-      <selection activeCell="C236" sqref="C236:E255"/>
+    <sheetView tabSelected="1" topLeftCell="A252" workbookViewId="0">
+      <selection activeCell="D271" sqref="C271:E275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8604,6 +8667,586 @@
         <v>15.747999999999999</v>
       </c>
       <c r="I255">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="256" spans="1:9">
+      <c r="A256" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B256" s="1">
+        <v>0.66875000000000007</v>
+      </c>
+      <c r="C256" s="2">
+        <v>11.12</v>
+      </c>
+      <c r="D256" s="2">
+        <v>3.25</v>
+      </c>
+      <c r="E256" s="2">
+        <v>38</v>
+      </c>
+      <c r="F256" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G256" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H256">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I256">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9">
+      <c r="A257" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B257" s="1">
+        <v>0.67152777777777783</v>
+      </c>
+      <c r="C257" s="2">
+        <v>11.9</v>
+      </c>
+      <c r="D257" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E257" s="2">
+        <v>27</v>
+      </c>
+      <c r="F257" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G257" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H257">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I257">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9">
+      <c r="A258" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B258" s="1">
+        <v>0.67291666666666661</v>
+      </c>
+      <c r="C258" s="2">
+        <v>10.11</v>
+      </c>
+      <c r="D258" s="2">
+        <v>12.05</v>
+      </c>
+      <c r="E258" s="2">
+        <v>32</v>
+      </c>
+      <c r="F258" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G258" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H258">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I258">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9">
+      <c r="A259" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B259" s="1">
+        <v>0.6743055555555556</v>
+      </c>
+      <c r="C259" s="2">
+        <v>11.23</v>
+      </c>
+      <c r="D259" s="2">
+        <v>6.89</v>
+      </c>
+      <c r="E259" s="2">
+        <v>117</v>
+      </c>
+      <c r="F259" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G259" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H259">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I259">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9">
+      <c r="A260" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B260" s="1">
+        <v>0.67569444444444438</v>
+      </c>
+      <c r="C260" s="2">
+        <v>11.73</v>
+      </c>
+      <c r="D260" s="2">
+        <v>25.73</v>
+      </c>
+      <c r="E260" s="3">
+        <v>11638</v>
+      </c>
+      <c r="F260" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G260" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H260">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I260">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9">
+      <c r="A261" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B261" s="1">
+        <v>0.86736111111111114</v>
+      </c>
+      <c r="C261" s="2">
+        <v>9.07</v>
+      </c>
+      <c r="D261" s="2">
+        <v>15.66</v>
+      </c>
+      <c r="E261" s="2">
+        <v>578</v>
+      </c>
+      <c r="F261" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G261" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H261">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I261">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9">
+      <c r="A262" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B262" s="1">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="C262" s="2">
+        <v>3.73</v>
+      </c>
+      <c r="D262" s="2">
+        <v>1.19</v>
+      </c>
+      <c r="E262" s="2">
+        <v>42</v>
+      </c>
+      <c r="F262" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G262" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H262">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I262">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9">
+      <c r="A263" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B263" s="1">
+        <v>0.86597222222222225</v>
+      </c>
+      <c r="C263" s="2">
+        <v>9.09</v>
+      </c>
+      <c r="D263" s="2">
+        <v>14.62</v>
+      </c>
+      <c r="E263" s="2">
+        <v>27</v>
+      </c>
+      <c r="F263" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G263" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H263">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I263">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9">
+      <c r="A264" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B264" s="1">
+        <v>0.86458333333333337</v>
+      </c>
+      <c r="C264" s="2">
+        <v>9.19</v>
+      </c>
+      <c r="D264" s="2">
+        <v>1.06</v>
+      </c>
+      <c r="E264" s="2">
+        <v>23</v>
+      </c>
+      <c r="F264" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G264" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H264">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I264">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9">
+      <c r="A265" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B265" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C265" s="2">
+        <v>9.1</v>
+      </c>
+      <c r="D265" s="2">
+        <v>6.37</v>
+      </c>
+      <c r="E265" s="2">
+        <v>27</v>
+      </c>
+      <c r="F265" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G265" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H265">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I265">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9">
+      <c r="A266" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B266" s="1">
+        <v>0.93263888888888891</v>
+      </c>
+      <c r="C266" s="2">
+        <v>11.64</v>
+      </c>
+      <c r="D266" s="2">
+        <v>23.05</v>
+      </c>
+      <c r="E266" s="2">
+        <v>27</v>
+      </c>
+      <c r="F266" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G266" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H266">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I266">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9">
+      <c r="A267" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B267" s="1">
+        <v>0.93055555555555547</v>
+      </c>
+      <c r="C267" s="2">
+        <v>11.17</v>
+      </c>
+      <c r="D267" s="2">
+        <v>1.08</v>
+      </c>
+      <c r="E267" s="2">
+        <v>28</v>
+      </c>
+      <c r="F267" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G267" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H267">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I267">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9">
+      <c r="A268" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B268" s="1">
+        <v>0.92569444444444438</v>
+      </c>
+      <c r="C268" s="2">
+        <v>7.48</v>
+      </c>
+      <c r="D268" s="2">
+        <v>17</v>
+      </c>
+      <c r="E268" s="2">
+        <v>31</v>
+      </c>
+      <c r="F268" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G268" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H268">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I268">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9">
+      <c r="A269" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B269" s="1">
+        <v>0.92361111111111116</v>
+      </c>
+      <c r="C269" s="2">
+        <v>11.24</v>
+      </c>
+      <c r="D269" s="2">
+        <v>20.73</v>
+      </c>
+      <c r="E269" s="2">
+        <v>44</v>
+      </c>
+      <c r="F269" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G269" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H269">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I269">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9">
+      <c r="A270" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B270" s="1">
+        <v>0.92083333333333339</v>
+      </c>
+      <c r="C270" s="2">
+        <v>10.82</v>
+      </c>
+      <c r="D270" s="2">
+        <v>1.77</v>
+      </c>
+      <c r="E270" s="2">
+        <v>25</v>
+      </c>
+      <c r="F270" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G270" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H270" s="10">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I270" s="10">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9">
+      <c r="A271" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B271" s="1">
+        <v>0.37222222222222223</v>
+      </c>
+      <c r="C271">
+        <v>9.42</v>
+      </c>
+      <c r="D271">
+        <v>0.99</v>
+      </c>
+      <c r="E271">
+        <v>37</v>
+      </c>
+      <c r="F271" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G271" t="s">
+        <v>16</v>
+      </c>
+      <c r="H271">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I271">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9">
+      <c r="A272" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B272" s="1">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="C272">
+        <v>8.9600000000000009</v>
+      </c>
+      <c r="D272">
+        <v>0.82</v>
+      </c>
+      <c r="E272">
+        <v>38</v>
+      </c>
+      <c r="F272" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G272" t="s">
+        <v>16</v>
+      </c>
+      <c r="H272">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I272">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9">
+      <c r="A273" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B273" s="1">
+        <v>0.36944444444444446</v>
+      </c>
+      <c r="C273">
+        <v>3.26</v>
+      </c>
+      <c r="D273">
+        <v>0.81</v>
+      </c>
+      <c r="E273">
+        <v>38</v>
+      </c>
+      <c r="F273" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G273" t="s">
+        <v>16</v>
+      </c>
+      <c r="H273">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I273">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9">
+      <c r="A274" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B274" s="1">
+        <v>0.36944444444444446</v>
+      </c>
+      <c r="C274">
+        <v>6.19</v>
+      </c>
+      <c r="D274">
+        <v>1.04</v>
+      </c>
+      <c r="E274">
+        <v>40</v>
+      </c>
+      <c r="F274" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G274" t="s">
+        <v>16</v>
+      </c>
+      <c r="H274">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I274">
+        <v>1.1020000000000001</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9">
+      <c r="A275" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B275" s="1">
+        <v>0.36874999999999997</v>
+      </c>
+      <c r="C275">
+        <v>7.81</v>
+      </c>
+      <c r="D275">
+        <v>0.7</v>
+      </c>
+      <c r="E275">
+        <v>45</v>
+      </c>
+      <c r="F275" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G275" t="s">
+        <v>16</v>
+      </c>
+      <c r="H275">
+        <v>15.747999999999999</v>
+      </c>
+      <c r="I275">
         <v>1.1020000000000001</v>
       </c>
     </row>

</xml_diff>